<commit_message>
[fubo.ding] #95 feature: generate MTB report excel
</commit_message>
<xml_diff>
--- a/src/main/resources/static/requisition/MTB_pt.xlsx
+++ b/src/main/resources/static/requisition/MTB_pt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinghan.xu/Desktop/XLS requisition template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fubo.ding/projects_siglus_to14/siglus-api/src/main/resources/static/requisition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922E9B7F-18A6-8943-93E6-4E9020F4FB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501D416D-350D-E94C-94D4-10D8BAEDA5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="500" windowWidth="34500" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="132">
   <si>
     <r>
       <rPr>
@@ -30,26 +30,6 @@
         <family val="2"/>
       </rPr>
       <t>Mapa Mensal de Medicamentos da TB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <rFont val="Arial MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>Cicloserina; 250mg; Caps</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <rFont val="Arial MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>comp</t>
     </r>
   </si>
   <si>
@@ -254,25 +234,10 @@
     </r>
   </si>
   <si>
-    <t>MAPUTO PROVINCIA</t>
-  </si>
-  <si>
-    <t>CIDADE DA MATOLA</t>
-  </si>
-  <si>
-    <t>DPM Maputo Província</t>
-  </si>
-  <si>
     <t>Balancente dos Medicamentos usados no tratamento e profilaxia da Tuberculose</t>
   </si>
   <si>
     <t>Sensível Intensiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dacruzmirole</t>
-  </si>
-  <si>
-    <t>09 Feb 2024</t>
   </si>
   <si>
     <t>REPÚBLICA DE MOÇAMBIQUE
@@ -292,9 +257,6 @@
     <t>Mês:</t>
   </si>
   <si>
-    <t>Janeiro</t>
-  </si>
-  <si>
     <t>Ano:</t>
   </si>
   <si>
@@ -434,16 +396,245 @@
   </si>
   <si>
     <t xml:space="preserve">Data de elaboração: </t>
+  </si>
+  <si>
+    <t>{provinceName}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{districtName}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{facilityName}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{month}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{year}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{productLineItem.productName}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{productLineItem.productUnit}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{productLineItem.productInitialStock}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{productLineItem.productEntries}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{productLineItem.productIssues}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{productLineItem.productAdjustments}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{productLineItem.productInventory}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{productLineItem.productExpireDate}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection0new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection0newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection0newColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection0total}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection1new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection1newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection1total}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn2}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn3}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn4}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn5}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn6}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn2}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn3}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn4}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn6}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn2}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn3}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn4}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn6}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenew}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn2}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn3}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn4}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypetotal}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{criança &gt; 25Kgprophylaxis}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{criança &gt; 25Kgtreatment}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{criança &lt; 25Kgprophylaxis}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{criança &lt; 25Kgtreatment}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{adultosprophylaxis}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{adultostreatment}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{createdDate}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> {authorize}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> {approve}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -560,6 +751,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -611,7 +808,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -749,15 +946,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -1071,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1084,64 +1272,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1150,7 +1320,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1171,49 +1341,49 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1222,47 +1392,23 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1270,13 +1416,31 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1288,135 +1452,126 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1520,9 +1675,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1560,9 +1715,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1595,9 +1750,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1630,9 +1802,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1808,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -1828,729 +2017,733 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="42" customHeight="1">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="96" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="102" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="14.5" customHeight="1">
+      <c r="A2" s="76"/>
+      <c r="B2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="98" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="14.5" customHeight="1">
+      <c r="A3" s="76"/>
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="93"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+    </row>
+    <row r="4" spans="1:11" ht="14" customHeight="1">
+      <c r="A4" s="76"/>
+      <c r="B4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="93"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+    </row>
+    <row r="5" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.5" customHeight="1">
+      <c r="B6" s="12"/>
+      <c r="C6" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="57"/>
+    </row>
+    <row r="7" spans="1:11" ht="31.5" customHeight="1">
+      <c r="B7" s="11"/>
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="19.5" customHeight="1">
+      <c r="C8" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28" customHeight="1">
+      <c r="A11" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="89" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="89"/>
+      <c r="D11" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="G11" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" ht="14" customHeight="1">
+      <c r="A12" s="82"/>
+      <c r="B12" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="84" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="14.5" customHeight="1">
-      <c r="A2" s="106"/>
-      <c r="B2" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="90" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="107">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="14.5" customHeight="1">
-      <c r="A3" s="106"/>
-      <c r="B3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="108"/>
-    </row>
-    <row r="4" spans="1:11" ht="14" customHeight="1">
-      <c r="A4" s="106"/>
-      <c r="B4" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="87"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="108"/>
-    </row>
-    <row r="5" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A5" s="102"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="104"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.5" customHeight="1">
-      <c r="B6" s="18"/>
-      <c r="C6" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="83"/>
-    </row>
-    <row r="7" spans="1:11" ht="31.5" customHeight="1">
-      <c r="B7" s="17"/>
-      <c r="C7" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="D12" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="G12" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="69"/>
+      <c r="J12" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="25"/>
+    </row>
+    <row r="13" spans="1:11" ht="13" customHeight="1">
+      <c r="A13" s="82"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="54"/>
+      <c r="J13" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" s="26"/>
+    </row>
+    <row r="14" spans="1:11" ht="13" customHeight="1">
+      <c r="A14" s="82"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="54"/>
+      <c r="J14" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="K14" s="26"/>
+    </row>
+    <row r="15" spans="1:11" ht="13" customHeight="1">
+      <c r="A15" s="82"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="54"/>
+      <c r="J15" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="K15" s="26"/>
+    </row>
+    <row r="16" spans="1:11" ht="13" customHeight="1">
+      <c r="A16" s="82"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="54"/>
+      <c r="J16" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="K16" s="26"/>
+    </row>
+    <row r="17" spans="1:11" ht="13" customHeight="1">
+      <c r="A17" s="82"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="54"/>
+      <c r="J17" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="K17" s="26"/>
+    </row>
+    <row r="18" spans="1:11" ht="13" customHeight="1">
+      <c r="A18" s="82"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="81"/>
+      <c r="J18" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" s="26"/>
+    </row>
+    <row r="19" spans="1:11" ht="13" customHeight="1">
+      <c r="A19" s="82"/>
+      <c r="B19" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="33"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="K19" s="26"/>
+    </row>
+    <row r="20" spans="1:11" ht="13" customHeight="1">
+      <c r="A20" s="82"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="33"/>
+      <c r="G20" s="28"/>
+      <c r="K20" s="25"/>
+    </row>
+    <row r="21" spans="1:11" ht="13" customHeight="1">
+      <c r="A21" s="82"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="33"/>
+      <c r="G21" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="69"/>
+      <c r="J21" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="26"/>
+    </row>
+    <row r="22" spans="1:11" ht="13" customHeight="1">
+      <c r="A22" s="82"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="33"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="54"/>
+      <c r="J22" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="K22" s="26"/>
+    </row>
+    <row r="23" spans="1:11" ht="13" customHeight="1">
+      <c r="A23" s="82"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="33"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="54"/>
+      <c r="J23" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="K23" s="26"/>
+    </row>
+    <row r="24" spans="1:11" ht="13" customHeight="1">
+      <c r="A24" s="82"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="33"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="54"/>
+      <c r="J24" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="K24" s="26"/>
+    </row>
+    <row r="25" spans="1:11" ht="13" customHeight="1">
+      <c r="A25" s="82"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="33"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="K25" s="25"/>
+    </row>
+    <row r="26" spans="1:11" ht="13" customHeight="1">
+      <c r="A26" s="46"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="34"/>
+      <c r="G26" s="28"/>
+      <c r="K26" s="26"/>
+    </row>
+    <row r="27" spans="1:11" ht="13" customHeight="1">
+      <c r="A27" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="19.5" customHeight="1">
-      <c r="C8" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="11">
-        <v>22100</v>
-      </c>
-      <c r="F8" s="11">
-        <v>8400</v>
-      </c>
-      <c r="G8" s="11">
-        <v>7300</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="11">
-        <v>23200</v>
-      </c>
-      <c r="J8" s="12">
-        <v>45565</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="28" customHeight="1">
-      <c r="A11" s="95" t="s">
+      <c r="D27" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="101" t="s">
+      <c r="E27" s="35"/>
+      <c r="G27" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27" s="69"/>
+      <c r="J27" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="26"/>
+    </row>
+    <row r="28" spans="1:11" ht="13" customHeight="1">
+      <c r="A28" s="51"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="33"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="I28" s="54"/>
+      <c r="J28" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="K28" s="26"/>
+    </row>
+    <row r="29" spans="1:11" ht="13" customHeight="1">
+      <c r="A29" s="51"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="33"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" s="54"/>
+      <c r="J29" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="K29" s="25"/>
+    </row>
+    <row r="30" spans="1:11" ht="13" customHeight="1">
+      <c r="A30" s="51"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="36"/>
+      <c r="F30" s="18"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="13" customHeight="1">
+      <c r="A31" s="51"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="33"/>
+      <c r="F31" s="18"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="23"/>
+    </row>
+    <row r="32" spans="1:11" ht="13" customHeight="1">
+      <c r="A32" s="51"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="33"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="67"/>
+    </row>
+    <row r="33" spans="1:10" ht="13" customHeight="1">
+      <c r="A33" s="51"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="33"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+    </row>
+    <row r="34" spans="1:10" ht="13" customHeight="1">
+      <c r="A34" s="51"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="33"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+    </row>
+    <row r="35" spans="1:10" ht="13" customHeight="1">
+      <c r="A35" s="51"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="33"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:10" ht="13" customHeight="1">
+      <c r="A36" s="52"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="19"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:10" ht="29" customHeight="1">
+      <c r="A38" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="101"/>
-      <c r="D11" s="47" t="s">
+      <c r="B38" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="G11" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="30"/>
-    </row>
-    <row r="12" spans="1:11" ht="14" customHeight="1">
-      <c r="A12" s="95"/>
-      <c r="B12" s="96" t="s">
+      <c r="C38" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="50">
-        <v>32968</v>
-      </c>
-      <c r="E12" s="39"/>
-      <c r="G12" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="79" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="77"/>
-      <c r="J12" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="31"/>
-    </row>
-    <row r="13" spans="1:11" ht="13" customHeight="1">
-      <c r="A13" s="95"/>
-      <c r="B13" s="97"/>
-      <c r="C13" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="50">
-        <v>32238</v>
-      </c>
-      <c r="E13" s="39"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="111" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="78"/>
-      <c r="J13" s="36">
-        <v>605</v>
-      </c>
-      <c r="K13" s="32"/>
-    </row>
-    <row r="14" spans="1:11" ht="13" customHeight="1">
-      <c r="A14" s="95"/>
-      <c r="B14" s="97"/>
-      <c r="C14" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="51">
-        <v>864</v>
-      </c>
-      <c r="E14" s="39"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="111" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="78"/>
-      <c r="J14" s="36">
-        <v>22</v>
-      </c>
-      <c r="K14" s="32"/>
-    </row>
-    <row r="15" spans="1:11" ht="13" customHeight="1">
-      <c r="A15" s="95"/>
-      <c r="B15" s="97"/>
-      <c r="C15" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="51">
-        <v>814</v>
-      </c>
-      <c r="E15" s="39"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="111" t="s">
-        <v>68</v>
-      </c>
-      <c r="I15" s="78"/>
-      <c r="J15" s="36">
-        <v>10</v>
-      </c>
-      <c r="K15" s="32"/>
-    </row>
-    <row r="16" spans="1:11" ht="13" customHeight="1">
-      <c r="A16" s="95"/>
-      <c r="B16" s="97"/>
-      <c r="C16" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="51">
-        <v>1003</v>
-      </c>
-      <c r="E16" s="39"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="111" t="s">
-        <v>69</v>
-      </c>
-      <c r="I16" s="78"/>
-      <c r="J16" s="36">
-        <v>52</v>
-      </c>
-      <c r="K16" s="32"/>
-    </row>
-    <row r="17" spans="1:11" ht="13" customHeight="1">
-      <c r="A17" s="95"/>
-      <c r="B17" s="97"/>
-      <c r="C17" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="51">
-        <v>3</v>
-      </c>
-      <c r="E17" s="39"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="111" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="78"/>
-      <c r="J17" s="36">
-        <v>0</v>
-      </c>
-      <c r="K17" s="32"/>
-    </row>
-    <row r="18" spans="1:11" ht="13" customHeight="1">
-      <c r="A18" s="95"/>
-      <c r="B18" s="98"/>
-      <c r="C18" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="51">
-        <v>80</v>
-      </c>
-      <c r="E18" s="39"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="112" t="s">
+      <c r="D38" s="44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="14" customHeight="1">
+      <c r="A39" s="51"/>
+      <c r="B39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="14" customHeight="1">
+      <c r="A40" s="51"/>
+      <c r="B40" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="42">
+      <c r="A41" s="51"/>
+      <c r="B41" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="47" customFormat="1" ht="28">
+      <c r="A43" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="I18" s="94"/>
-      <c r="J18" s="36">
-        <v>1</v>
-      </c>
-      <c r="K18" s="32"/>
-    </row>
-    <row r="19" spans="1:11" ht="13" customHeight="1">
-      <c r="A19" s="95"/>
-      <c r="B19" s="109" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="52">
-        <v>2092</v>
-      </c>
-      <c r="E19" s="39"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="36">
-        <v>690</v>
-      </c>
-      <c r="K19" s="32"/>
-    </row>
-    <row r="20" spans="1:11" ht="13" customHeight="1">
-      <c r="A20" s="95"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="52">
-        <v>2215</v>
-      </c>
-      <c r="E20" s="39"/>
-      <c r="G20" s="34"/>
-      <c r="K20" s="31"/>
-    </row>
-    <row r="21" spans="1:11" ht="13" customHeight="1">
-      <c r="A21" s="95"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="52">
-        <v>411</v>
-      </c>
-      <c r="E21" s="39"/>
-      <c r="G21" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21" s="77"/>
-      <c r="J21" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" s="32"/>
-    </row>
-    <row r="22" spans="1:11" ht="13" customHeight="1">
-      <c r="A22" s="95"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="52">
-        <v>21</v>
-      </c>
-      <c r="E22" s="39"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="111" t="s">
+      <c r="B43" s="99" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="I22" s="78"/>
-      <c r="J22" s="36">
-        <v>1098</v>
-      </c>
-      <c r="K22" s="32"/>
-    </row>
-    <row r="23" spans="1:11" ht="13" customHeight="1">
-      <c r="A23" s="95"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="52">
-        <v>26</v>
-      </c>
-      <c r="E23" s="39"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="111" t="s">
+      <c r="E43" s="99" t="s">
+        <v>131</v>
+      </c>
+      <c r="G43" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="I23" s="78"/>
-      <c r="J23" s="36">
-        <v>2760</v>
-      </c>
-      <c r="K23" s="32"/>
-    </row>
-    <row r="24" spans="1:11" ht="13" customHeight="1">
-      <c r="A24" s="95"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="52">
-        <v>0</v>
-      </c>
-      <c r="E24" s="39"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="111" t="s">
-        <v>74</v>
-      </c>
-      <c r="I24" s="78"/>
-      <c r="J24" s="36">
-        <v>470</v>
-      </c>
-      <c r="K24" s="32"/>
-    </row>
-    <row r="25" spans="1:11" ht="13" customHeight="1">
-      <c r="A25" s="95"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="52">
-        <v>11</v>
-      </c>
-      <c r="E25" s="39"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="36">
-        <v>4328</v>
-      </c>
-      <c r="K25" s="31"/>
-    </row>
-    <row r="26" spans="1:11" ht="13" customHeight="1">
-      <c r="A26" s="55"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="40"/>
-      <c r="G26" s="34"/>
-      <c r="K26" s="32"/>
-    </row>
-    <row r="27" spans="1:11" ht="13" customHeight="1">
-      <c r="A27" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="110" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="41"/>
-      <c r="G27" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="I27" s="77"/>
-      <c r="J27" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="K27" s="32"/>
-    </row>
-    <row r="28" spans="1:11" ht="13" customHeight="1">
-      <c r="A28" s="65"/>
-      <c r="B28" s="92"/>
-      <c r="C28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="4">
-        <v>15207</v>
-      </c>
-      <c r="E28" s="39"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="113" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" s="78"/>
-      <c r="J28" s="36">
-        <v>4315</v>
-      </c>
-      <c r="K28" s="32"/>
-    </row>
-    <row r="29" spans="1:11" ht="13" customHeight="1">
-      <c r="A29" s="65"/>
-      <c r="B29" s="92"/>
-      <c r="C29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="4">
-        <v>26300</v>
-      </c>
-      <c r="E29" s="39"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="113" t="s">
-        <v>77</v>
-      </c>
-      <c r="I29" s="78"/>
-      <c r="J29" s="36">
-        <v>429</v>
-      </c>
-      <c r="K29" s="31"/>
-    </row>
-    <row r="30" spans="1:11" ht="13" customHeight="1">
-      <c r="A30" s="65"/>
-      <c r="B30" s="92"/>
-      <c r="C30" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="4">
-        <v>280</v>
-      </c>
-      <c r="E30" s="42"/>
-      <c r="F30" s="24"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="37">
-        <v>4744</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="13" customHeight="1">
-      <c r="A31" s="65"/>
-      <c r="B31" s="92"/>
-      <c r="C31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="4">
-        <v>4788</v>
-      </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="24"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="29"/>
-    </row>
-    <row r="32" spans="1:11" ht="13" customHeight="1">
-      <c r="A32" s="65"/>
-      <c r="B32" s="92"/>
-      <c r="C32" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="4">
-        <v>41737</v>
-      </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="75"/>
-    </row>
-    <row r="33" spans="1:10" ht="13" customHeight="1">
-      <c r="A33" s="65"/>
-      <c r="B33" s="92"/>
-      <c r="C33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="4">
-        <v>1452</v>
-      </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-    </row>
-    <row r="34" spans="1:10" ht="13" customHeight="1">
-      <c r="A34" s="65"/>
-      <c r="B34" s="92"/>
-      <c r="C34" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="4">
-        <v>800</v>
-      </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-    </row>
-    <row r="35" spans="1:10" ht="13" customHeight="1">
-      <c r="A35" s="65"/>
-      <c r="B35" s="92"/>
-      <c r="C35" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="4">
-        <v>67188</v>
-      </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="24"/>
-    </row>
-    <row r="36" spans="1:10" ht="13" customHeight="1">
-      <c r="A36" s="80"/>
-      <c r="B36" s="93"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="24"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="25"/>
-      <c r="F37" s="24"/>
-    </row>
-    <row r="38" spans="1:10" ht="29" customHeight="1">
-      <c r="A38" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="14" customHeight="1">
-      <c r="A39" s="65"/>
-      <c r="B39" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="2">
-        <v>3819</v>
-      </c>
-      <c r="D39" s="54">
-        <v>3869</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="14" customHeight="1">
-      <c r="A40" s="65"/>
-      <c r="B40" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="2">
-        <v>261</v>
-      </c>
-      <c r="D40" s="54">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="28">
-      <c r="A41" s="65"/>
-      <c r="B41" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="2">
-        <v>128</v>
-      </c>
-      <c r="D41" s="54">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="56" customFormat="1" ht="42">
-      <c r="A43" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="H43" s="58" t="s">
-        <v>28</v>
+      <c r="H43" s="101" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="J2:J4"/>
     <mergeCell ref="B27:B36"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="A11:A25"/>
     <mergeCell ref="B12:B18"/>
     <mergeCell ref="B19:B25"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="J2:J4"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I2:I4"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A27:A36"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="C6:J6"/>
@@ -2566,11 +2759,8 @@
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A27:A36"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[fubo.ding] #95 refactor: update template excel sheet name to MTB
</commit_message>
<xml_diff>
--- a/src/main/resources/static/requisition/MTB_pt.xlsx
+++ b/src/main/resources/static/requisition/MTB_pt.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fubo.ding/projects_siglus_to14/siglus-api/src/main/resources/static/requisition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501D416D-350D-E94C-94D4-10D8BAEDA5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C90B6F-96E4-3246-9D3A-130AB97BC1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="500" windowWidth="34500" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1" sheetId="1" r:id="rId1"/>
+    <sheet name="MTB" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -1410,6 +1410,111 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1419,12 +1524,6 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1467,107 +1566,8 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1997,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -2024,17 +2024,17 @@
       <c r="C1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="96" t="s">
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="102" t="s">
+      <c r="J1" s="51" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2046,15 +2046,15 @@
       <c r="C2" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="97" t="s">
+      <c r="D2" s="81"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="98" t="s">
+      <c r="J2" s="77" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2066,13 +2066,13 @@
       <c r="C3" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
     </row>
     <row r="4" spans="1:11" ht="14" customHeight="1">
       <c r="A4" s="76"/>
@@ -2082,13 +2082,13 @@
       <c r="C4" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="93"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="72"/>
@@ -2104,16 +2104,16 @@
     </row>
     <row r="6" spans="1:11" ht="16.5" customHeight="1">
       <c r="B6" s="12"/>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="57"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="90"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" customHeight="1">
       <c r="B7" s="11"/>
@@ -2169,28 +2169,28 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="28" customHeight="1">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="89"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="41" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="32"/>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="60"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="93"/>
       <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" ht="14" customHeight="1">
-      <c r="A12" s="82"/>
-      <c r="B12" s="83" t="s">
+      <c r="A12" s="60"/>
+      <c r="B12" s="61" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="40" t="s">
@@ -2200,10 +2200,10 @@
         <v>102</v>
       </c>
       <c r="E12" s="33"/>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="68" t="s">
         <v>56</v>
       </c>
       <c r="I12" s="69"/>
@@ -2213,8 +2213,8 @@
       <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:11" ht="13" customHeight="1">
-      <c r="A13" s="82"/>
-      <c r="B13" s="84"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="62"/>
       <c r="C13" s="40" t="s">
         <v>2</v>
       </c>
@@ -2222,19 +2222,19 @@
         <v>108</v>
       </c>
       <c r="E13" s="33"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="53" t="s">
+      <c r="G13" s="95"/>
+      <c r="H13" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="54"/>
+      <c r="I13" s="71"/>
       <c r="J13" s="30" t="s">
         <v>116</v>
       </c>
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" ht="13" customHeight="1">
-      <c r="A14" s="82"/>
-      <c r="B14" s="84"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="40" t="s">
         <v>3</v>
       </c>
@@ -2242,19 +2242,19 @@
         <v>103</v>
       </c>
       <c r="E14" s="33"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="53" t="s">
+      <c r="G14" s="95"/>
+      <c r="H14" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="54"/>
+      <c r="I14" s="71"/>
       <c r="J14" s="30" t="s">
         <v>117</v>
       </c>
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="13" customHeight="1">
-      <c r="A15" s="82"/>
-      <c r="B15" s="84"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="62"/>
       <c r="C15" s="40" t="s">
         <v>4</v>
       </c>
@@ -2262,19 +2262,19 @@
         <v>104</v>
       </c>
       <c r="E15" s="33"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="53" t="s">
+      <c r="G15" s="95"/>
+      <c r="H15" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="54"/>
+      <c r="I15" s="71"/>
       <c r="J15" s="30" t="s">
         <v>118</v>
       </c>
       <c r="K15" s="26"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1">
-      <c r="A16" s="82"/>
-      <c r="B16" s="84"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="62"/>
       <c r="C16" s="40" t="s">
         <v>5</v>
       </c>
@@ -2282,19 +2282,19 @@
         <v>105</v>
       </c>
       <c r="E16" s="33"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="53" t="s">
+      <c r="G16" s="95"/>
+      <c r="H16" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="54"/>
+      <c r="I16" s="71"/>
       <c r="J16" s="30" t="s">
         <v>119</v>
       </c>
       <c r="K16" s="26"/>
     </row>
     <row r="17" spans="1:11" ht="13" customHeight="1">
-      <c r="A17" s="82"/>
-      <c r="B17" s="84"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="62"/>
       <c r="C17" s="40" t="s">
         <v>6</v>
       </c>
@@ -2302,19 +2302,19 @@
         <v>106</v>
       </c>
       <c r="E17" s="33"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="53" t="s">
+      <c r="G17" s="95"/>
+      <c r="H17" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="54"/>
+      <c r="I17" s="71"/>
       <c r="J17" s="30" t="s">
         <v>120</v>
       </c>
       <c r="K17" s="26"/>
     </row>
     <row r="18" spans="1:11" ht="13" customHeight="1">
-      <c r="A18" s="82"/>
-      <c r="B18" s="85"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="40" t="s">
         <v>7</v>
       </c>
@@ -2322,19 +2322,19 @@
         <v>107</v>
       </c>
       <c r="E18" s="33"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="80" t="s">
+      <c r="G18" s="96"/>
+      <c r="H18" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="81"/>
+      <c r="I18" s="59"/>
       <c r="J18" s="30" t="s">
         <v>121</v>
       </c>
       <c r="K18" s="26"/>
     </row>
     <row r="19" spans="1:11" ht="13" customHeight="1">
-      <c r="A19" s="82"/>
-      <c r="B19" s="86" t="s">
+      <c r="A19" s="60"/>
+      <c r="B19" s="64" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="39" t="s">
@@ -2355,8 +2355,8 @@
       <c r="K19" s="26"/>
     </row>
     <row r="20" spans="1:11" ht="13" customHeight="1">
-      <c r="A20" s="82"/>
-      <c r="B20" s="87"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="39" t="s">
         <v>2</v>
       </c>
@@ -2368,8 +2368,8 @@
       <c r="K20" s="25"/>
     </row>
     <row r="21" spans="1:11" ht="13" customHeight="1">
-      <c r="A21" s="82"/>
-      <c r="B21" s="87"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="39" t="s">
         <v>3</v>
       </c>
@@ -2377,10 +2377,10 @@
         <v>110</v>
       </c>
       <c r="E21" s="33"/>
-      <c r="G21" s="61" t="s">
+      <c r="G21" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="71" t="s">
+      <c r="H21" s="68" t="s">
         <v>57</v>
       </c>
       <c r="I21" s="69"/>
@@ -2390,8 +2390,8 @@
       <c r="K21" s="26"/>
     </row>
     <row r="22" spans="1:11" ht="13" customHeight="1">
-      <c r="A22" s="82"/>
-      <c r="B22" s="87"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="39" t="s">
         <v>4</v>
       </c>
@@ -2399,19 +2399,19 @@
         <v>111</v>
       </c>
       <c r="E22" s="33"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="53" t="s">
+      <c r="G22" s="95"/>
+      <c r="H22" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="I22" s="54"/>
+      <c r="I22" s="71"/>
       <c r="J22" s="30" t="s">
         <v>87</v>
       </c>
       <c r="K22" s="26"/>
     </row>
     <row r="23" spans="1:11" ht="13" customHeight="1">
-      <c r="A23" s="82"/>
-      <c r="B23" s="87"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="39" t="s">
         <v>5</v>
       </c>
@@ -2419,19 +2419,19 @@
         <v>112</v>
       </c>
       <c r="E23" s="33"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="53" t="s">
+      <c r="G23" s="95"/>
+      <c r="H23" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="I23" s="54"/>
+      <c r="I23" s="71"/>
       <c r="J23" s="30" t="s">
         <v>88</v>
       </c>
       <c r="K23" s="26"/>
     </row>
     <row r="24" spans="1:11" ht="13" customHeight="1">
-      <c r="A24" s="82"/>
-      <c r="B24" s="87"/>
+      <c r="A24" s="60"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="39" t="s">
         <v>7</v>
       </c>
@@ -2439,19 +2439,19 @@
         <v>113</v>
       </c>
       <c r="E24" s="33"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="53" t="s">
+      <c r="G24" s="95"/>
+      <c r="H24" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="I24" s="54"/>
+      <c r="I24" s="71"/>
       <c r="J24" s="30" t="s">
         <v>89</v>
       </c>
       <c r="K24" s="26"/>
     </row>
     <row r="25" spans="1:11" ht="13" customHeight="1">
-      <c r="A25" s="82"/>
-      <c r="B25" s="88"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="39" t="s">
         <v>8</v>
       </c>
@@ -2479,10 +2479,10 @@
       <c r="K26" s="26"/>
     </row>
     <row r="27" spans="1:11" ht="13" customHeight="1">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="55" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="42" t="s">
@@ -2492,10 +2492,10 @@
         <v>44</v>
       </c>
       <c r="E27" s="35"/>
-      <c r="G27" s="64" t="s">
+      <c r="G27" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="68" t="s">
+      <c r="H27" s="101" t="s">
         <v>67</v>
       </c>
       <c r="I27" s="69"/>
@@ -2505,8 +2505,8 @@
       <c r="K27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="13" customHeight="1">
-      <c r="A28" s="51"/>
-      <c r="B28" s="78"/>
+      <c r="A28" s="86"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
@@ -2514,19 +2514,19 @@
         <v>94</v>
       </c>
       <c r="E28" s="33"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="70" t="s">
+      <c r="G28" s="97"/>
+      <c r="H28" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="54"/>
+      <c r="I28" s="71"/>
       <c r="J28" s="30" t="s">
         <v>91</v>
       </c>
       <c r="K28" s="26"/>
     </row>
     <row r="29" spans="1:11" ht="13" customHeight="1">
-      <c r="A29" s="51"/>
-      <c r="B29" s="78"/>
+      <c r="A29" s="86"/>
+      <c r="B29" s="56"/>
       <c r="C29" s="4" t="s">
         <v>10</v>
       </c>
@@ -2534,19 +2534,19 @@
         <v>95</v>
       </c>
       <c r="E29" s="33"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="70" t="s">
+      <c r="G29" s="97"/>
+      <c r="H29" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="54"/>
+      <c r="I29" s="71"/>
       <c r="J29" s="30" t="s">
         <v>92</v>
       </c>
       <c r="K29" s="25"/>
     </row>
     <row r="30" spans="1:11" ht="13" customHeight="1">
-      <c r="A30" s="51"/>
-      <c r="B30" s="78"/>
+      <c r="A30" s="86"/>
+      <c r="B30" s="56"/>
       <c r="C30" s="21" t="s">
         <v>11</v>
       </c>
@@ -2564,8 +2564,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="13" customHeight="1">
-      <c r="A31" s="51"/>
-      <c r="B31" s="78"/>
+      <c r="A31" s="86"/>
+      <c r="B31" s="56"/>
       <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
@@ -2579,8 +2579,8 @@
       <c r="J31" s="23"/>
     </row>
     <row r="32" spans="1:11" ht="13" customHeight="1">
-      <c r="A32" s="51"/>
-      <c r="B32" s="78"/>
+      <c r="A32" s="86"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
@@ -2589,16 +2589,16 @@
       </c>
       <c r="E32" s="33"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="65" t="s">
+      <c r="G32" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="67"/>
+      <c r="H32" s="99"/>
+      <c r="I32" s="99"/>
+      <c r="J32" s="100"/>
     </row>
     <row r="33" spans="1:10" ht="13" customHeight="1">
-      <c r="A33" s="51"/>
-      <c r="B33" s="78"/>
+      <c r="A33" s="86"/>
+      <c r="B33" s="56"/>
       <c r="C33" s="4" t="s">
         <v>14</v>
       </c>
@@ -2613,8 +2613,8 @@
       <c r="J33" s="18"/>
     </row>
     <row r="34" spans="1:10" ht="13" customHeight="1">
-      <c r="A34" s="51"/>
-      <c r="B34" s="78"/>
+      <c r="A34" s="86"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="4" t="s">
         <v>15</v>
       </c>
@@ -2629,8 +2629,8 @@
       <c r="J34" s="18"/>
     </row>
     <row r="35" spans="1:10" ht="13" customHeight="1">
-      <c r="A35" s="51"/>
-      <c r="B35" s="78"/>
+      <c r="A35" s="86"/>
+      <c r="B35" s="56"/>
       <c r="C35" s="4" t="s">
         <v>16</v>
       </c>
@@ -2641,8 +2641,8 @@
       <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:10" ht="13" customHeight="1">
-      <c r="A36" s="52"/>
-      <c r="B36" s="79"/>
+      <c r="A36" s="87"/>
+      <c r="B36" s="57"/>
       <c r="C36" s="20"/>
       <c r="D36" s="3"/>
       <c r="E36" s="37"/>
@@ -2653,7 +2653,7 @@
       <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:10" ht="29" customHeight="1">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="85" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="42" t="s">
@@ -2667,7 +2667,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="14" customHeight="1">
-      <c r="A39" s="51"/>
+      <c r="A39" s="86"/>
       <c r="B39" s="4" t="s">
         <v>49</v>
       </c>
@@ -2679,7 +2679,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="14" customHeight="1">
-      <c r="A40" s="51"/>
+      <c r="A40" s="86"/>
       <c r="B40" s="4" t="s">
         <v>50</v>
       </c>
@@ -2691,7 +2691,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="42">
-      <c r="A41" s="51"/>
+      <c r="A41" s="86"/>
       <c r="B41" s="4" t="s">
         <v>51</v>
       </c>
@@ -2703,49 +2703,27 @@
       </c>
     </row>
     <row r="43" spans="1:10" s="47" customFormat="1" ht="28">
-      <c r="A43" s="99" t="s">
+      <c r="A43" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="99" t="s">
+      <c r="B43" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="99" t="s">
+      <c r="D43" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="E43" s="99" t="s">
+      <c r="E43" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="G43" s="100" t="s">
+      <c r="G43" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="H43" s="101" t="s">
+      <c r="H43" s="54" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B27:B36"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="A11:A25"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="G11:J11"/>
@@ -2759,6 +2737,28 @@
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="B27:B36"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="A11:A25"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[fubo.ding] #116&117 bugfix: update excel template
</commit_message>
<xml_diff>
--- a/src/main/resources/static/requisition/MTB_pt.xlsx
+++ b/src/main/resources/static/requisition/MTB_pt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fubo.ding/projects_siglus_to14/siglus-api/src/main/resources/static/requisition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C90B6F-96E4-3246-9D3A-130AB97BC1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53E27E9-4FBE-4E41-A54D-9D2763ECBAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="500" windowWidth="34500" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="133">
   <si>
     <r>
       <rPr>
@@ -627,6 +627,10 @@
   </si>
   <si>
     <t xml:space="preserve"> {approve}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{comment}</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
@@ -1259,7 +1263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1425,6 +1429,108 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1464,110 +1570,14 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1997,8 +2007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -2017,20 +2027,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="42" customHeight="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="79" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="80"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="84"/>
       <c r="I1" s="50" t="s">
         <v>26</v>
       </c>
@@ -2039,81 +2049,81 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.5" customHeight="1">
-      <c r="A2" s="76"/>
+      <c r="A2" s="80"/>
       <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="84" t="s">
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="77" t="s">
+      <c r="J2" s="81" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.5" customHeight="1">
-      <c r="A3" s="76"/>
+      <c r="A3" s="80"/>
       <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
     </row>
     <row r="4" spans="1:11" ht="14" customHeight="1">
-      <c r="A4" s="76"/>
+      <c r="A4" s="80"/>
       <c r="B4" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A5" s="72"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="74"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="78"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" customHeight="1">
       <c r="B6" s="12"/>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="90"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="57"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" customHeight="1">
       <c r="B7" s="11"/>
@@ -2169,28 +2179,28 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="28" customHeight="1">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="101"/>
       <c r="D11" s="41" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="32"/>
-      <c r="G11" s="91" t="s">
+      <c r="G11" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="93"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="62"/>
       <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" ht="14" customHeight="1">
-      <c r="A12" s="60"/>
-      <c r="B12" s="61" t="s">
+      <c r="A12" s="94"/>
+      <c r="B12" s="95" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="40" t="s">
@@ -2200,21 +2210,21 @@
         <v>102</v>
       </c>
       <c r="E12" s="33"/>
-      <c r="G12" s="94" t="s">
+      <c r="G12" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="69"/>
+      <c r="I12" s="71"/>
       <c r="J12" s="48" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:11" ht="13" customHeight="1">
-      <c r="A13" s="60"/>
-      <c r="B13" s="62"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="96"/>
       <c r="C13" s="40" t="s">
         <v>2</v>
       </c>
@@ -2222,19 +2232,19 @@
         <v>108</v>
       </c>
       <c r="E13" s="33"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="70" t="s">
+      <c r="G13" s="64"/>
+      <c r="H13" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="71"/>
+      <c r="I13" s="73"/>
       <c r="J13" s="30" t="s">
         <v>116</v>
       </c>
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" ht="13" customHeight="1">
-      <c r="A14" s="60"/>
-      <c r="B14" s="62"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="96"/>
       <c r="C14" s="40" t="s">
         <v>3</v>
       </c>
@@ -2242,19 +2252,19 @@
         <v>103</v>
       </c>
       <c r="E14" s="33"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="70" t="s">
+      <c r="G14" s="64"/>
+      <c r="H14" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="71"/>
+      <c r="I14" s="73"/>
       <c r="J14" s="30" t="s">
         <v>117</v>
       </c>
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="13" customHeight="1">
-      <c r="A15" s="60"/>
-      <c r="B15" s="62"/>
+      <c r="A15" s="94"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="40" t="s">
         <v>4</v>
       </c>
@@ -2262,19 +2272,19 @@
         <v>104</v>
       </c>
       <c r="E15" s="33"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="70" t="s">
+      <c r="G15" s="64"/>
+      <c r="H15" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="71"/>
+      <c r="I15" s="73"/>
       <c r="J15" s="30" t="s">
         <v>118</v>
       </c>
       <c r="K15" s="26"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1">
-      <c r="A16" s="60"/>
-      <c r="B16" s="62"/>
+      <c r="A16" s="94"/>
+      <c r="B16" s="96"/>
       <c r="C16" s="40" t="s">
         <v>5</v>
       </c>
@@ -2282,19 +2292,19 @@
         <v>105</v>
       </c>
       <c r="E16" s="33"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="70" t="s">
+      <c r="G16" s="64"/>
+      <c r="H16" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="71"/>
+      <c r="I16" s="73"/>
       <c r="J16" s="30" t="s">
         <v>119</v>
       </c>
       <c r="K16" s="26"/>
     </row>
     <row r="17" spans="1:11" ht="13" customHeight="1">
-      <c r="A17" s="60"/>
-      <c r="B17" s="62"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="96"/>
       <c r="C17" s="40" t="s">
         <v>6</v>
       </c>
@@ -2302,19 +2312,19 @@
         <v>106</v>
       </c>
       <c r="E17" s="33"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="70" t="s">
+      <c r="G17" s="64"/>
+      <c r="H17" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="71"/>
+      <c r="I17" s="73"/>
       <c r="J17" s="30" t="s">
         <v>120</v>
       </c>
       <c r="K17" s="26"/>
     </row>
     <row r="18" spans="1:11" ht="13" customHeight="1">
-      <c r="A18" s="60"/>
-      <c r="B18" s="63"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="97"/>
       <c r="C18" s="40" t="s">
         <v>7</v>
       </c>
@@ -2322,19 +2332,19 @@
         <v>107</v>
       </c>
       <c r="E18" s="33"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="58" t="s">
+      <c r="G18" s="65"/>
+      <c r="H18" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="59"/>
+      <c r="I18" s="93"/>
       <c r="J18" s="30" t="s">
         <v>121</v>
       </c>
       <c r="K18" s="26"/>
     </row>
     <row r="19" spans="1:11" ht="13" customHeight="1">
-      <c r="A19" s="60"/>
-      <c r="B19" s="64" t="s">
+      <c r="A19" s="94"/>
+      <c r="B19" s="98" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="39" t="s">
@@ -2355,8 +2365,8 @@
       <c r="K19" s="26"/>
     </row>
     <row r="20" spans="1:11" ht="13" customHeight="1">
-      <c r="A20" s="60"/>
-      <c r="B20" s="65"/>
+      <c r="A20" s="94"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="39" t="s">
         <v>2</v>
       </c>
@@ -2368,8 +2378,8 @@
       <c r="K20" s="25"/>
     </row>
     <row r="21" spans="1:11" ht="13" customHeight="1">
-      <c r="A21" s="60"/>
-      <c r="B21" s="65"/>
+      <c r="A21" s="94"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="39" t="s">
         <v>3</v>
       </c>
@@ -2377,21 +2387,21 @@
         <v>110</v>
       </c>
       <c r="E21" s="33"/>
-      <c r="G21" s="94" t="s">
+      <c r="G21" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="68" t="s">
+      <c r="H21" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="69"/>
+      <c r="I21" s="71"/>
       <c r="J21" s="48" t="s">
         <v>17</v>
       </c>
       <c r="K21" s="26"/>
     </row>
     <row r="22" spans="1:11" ht="13" customHeight="1">
-      <c r="A22" s="60"/>
-      <c r="B22" s="65"/>
+      <c r="A22" s="94"/>
+      <c r="B22" s="99"/>
       <c r="C22" s="39" t="s">
         <v>4</v>
       </c>
@@ -2399,19 +2409,19 @@
         <v>111</v>
       </c>
       <c r="E22" s="33"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="70" t="s">
+      <c r="G22" s="64"/>
+      <c r="H22" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="I22" s="71"/>
+      <c r="I22" s="73"/>
       <c r="J22" s="30" t="s">
         <v>87</v>
       </c>
       <c r="K22" s="26"/>
     </row>
     <row r="23" spans="1:11" ht="13" customHeight="1">
-      <c r="A23" s="60"/>
-      <c r="B23" s="65"/>
+      <c r="A23" s="94"/>
+      <c r="B23" s="99"/>
       <c r="C23" s="39" t="s">
         <v>5</v>
       </c>
@@ -2419,19 +2429,19 @@
         <v>112</v>
       </c>
       <c r="E23" s="33"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="70" t="s">
+      <c r="G23" s="64"/>
+      <c r="H23" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="I23" s="71"/>
+      <c r="I23" s="73"/>
       <c r="J23" s="30" t="s">
         <v>88</v>
       </c>
       <c r="K23" s="26"/>
     </row>
     <row r="24" spans="1:11" ht="13" customHeight="1">
-      <c r="A24" s="60"/>
-      <c r="B24" s="65"/>
+      <c r="A24" s="94"/>
+      <c r="B24" s="99"/>
       <c r="C24" s="39" t="s">
         <v>7</v>
       </c>
@@ -2439,19 +2449,19 @@
         <v>113</v>
       </c>
       <c r="E24" s="33"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="70" t="s">
+      <c r="G24" s="64"/>
+      <c r="H24" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="I24" s="71"/>
+      <c r="I24" s="73"/>
       <c r="J24" s="30" t="s">
         <v>89</v>
       </c>
       <c r="K24" s="26"/>
     </row>
     <row r="25" spans="1:11" ht="13" customHeight="1">
-      <c r="A25" s="60"/>
-      <c r="B25" s="66"/>
+      <c r="A25" s="94"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="39" t="s">
         <v>8</v>
       </c>
@@ -2479,10 +2489,10 @@
       <c r="K26" s="26"/>
     </row>
     <row r="27" spans="1:11" ht="13" customHeight="1">
-      <c r="A27" s="85" t="s">
+      <c r="A27" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="89" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="42" t="s">
@@ -2492,21 +2502,21 @@
         <v>44</v>
       </c>
       <c r="E27" s="35"/>
-      <c r="G27" s="97" t="s">
+      <c r="G27" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="101" t="s">
+      <c r="H27" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="I27" s="69"/>
+      <c r="I27" s="71"/>
       <c r="J27" s="48" t="s">
         <v>17</v>
       </c>
       <c r="K27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="13" customHeight="1">
-      <c r="A28" s="86"/>
-      <c r="B28" s="56"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="90"/>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
@@ -2514,19 +2524,19 @@
         <v>94</v>
       </c>
       <c r="E28" s="33"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="102" t="s">
+      <c r="G28" s="66"/>
+      <c r="H28" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="71"/>
+      <c r="I28" s="73"/>
       <c r="J28" s="30" t="s">
         <v>91</v>
       </c>
       <c r="K28" s="26"/>
     </row>
     <row r="29" spans="1:11" ht="13" customHeight="1">
-      <c r="A29" s="86"/>
-      <c r="B29" s="56"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="90"/>
       <c r="C29" s="4" t="s">
         <v>10</v>
       </c>
@@ -2534,19 +2544,19 @@
         <v>95</v>
       </c>
       <c r="E29" s="33"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="102" t="s">
+      <c r="G29" s="66"/>
+      <c r="H29" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="71"/>
+      <c r="I29" s="73"/>
       <c r="J29" s="30" t="s">
         <v>92</v>
       </c>
       <c r="K29" s="25"/>
     </row>
     <row r="30" spans="1:11" ht="13" customHeight="1">
-      <c r="A30" s="86"/>
-      <c r="B30" s="56"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="90"/>
       <c r="C30" s="21" t="s">
         <v>11</v>
       </c>
@@ -2564,8 +2574,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="13" customHeight="1">
-      <c r="A31" s="86"/>
-      <c r="B31" s="56"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="90"/>
       <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
@@ -2579,8 +2589,8 @@
       <c r="J31" s="23"/>
     </row>
     <row r="32" spans="1:11" ht="13" customHeight="1">
-      <c r="A32" s="86"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="59"/>
+      <c r="B32" s="90"/>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
@@ -2589,16 +2599,16 @@
       </c>
       <c r="E32" s="33"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="98" t="s">
+      <c r="G32" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="99"/>
-      <c r="I32" s="99"/>
-      <c r="J32" s="100"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="69"/>
     </row>
     <row r="33" spans="1:10" ht="13" customHeight="1">
-      <c r="A33" s="86"/>
-      <c r="B33" s="56"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="90"/>
       <c r="C33" s="4" t="s">
         <v>14</v>
       </c>
@@ -2607,14 +2617,16 @@
       </c>
       <c r="E33" s="33"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
+      <c r="G33" s="104" t="s">
+        <v>132</v>
+      </c>
+      <c r="H33" s="103"/>
+      <c r="I33" s="103"/>
+      <c r="J33" s="103"/>
     </row>
     <row r="34" spans="1:10" ht="13" customHeight="1">
-      <c r="A34" s="86"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="90"/>
       <c r="C34" s="4" t="s">
         <v>15</v>
       </c>
@@ -2629,8 +2641,8 @@
       <c r="J34" s="18"/>
     </row>
     <row r="35" spans="1:10" ht="13" customHeight="1">
-      <c r="A35" s="86"/>
-      <c r="B35" s="56"/>
+      <c r="A35" s="59"/>
+      <c r="B35" s="90"/>
       <c r="C35" s="4" t="s">
         <v>16</v>
       </c>
@@ -2641,8 +2653,8 @@
       <c r="F35" s="18"/>
     </row>
     <row r="36" spans="1:10" ht="13" customHeight="1">
-      <c r="A36" s="87"/>
-      <c r="B36" s="57"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="91"/>
       <c r="C36" s="20"/>
       <c r="D36" s="3"/>
       <c r="E36" s="37"/>
@@ -2653,7 +2665,7 @@
       <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:10" ht="29" customHeight="1">
-      <c r="A38" s="85" t="s">
+      <c r="A38" s="58" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="42" t="s">
@@ -2667,7 +2679,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="14" customHeight="1">
-      <c r="A39" s="86"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="4" t="s">
         <v>49</v>
       </c>
@@ -2679,7 +2691,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="14" customHeight="1">
-      <c r="A40" s="86"/>
+      <c r="A40" s="59"/>
       <c r="B40" s="4" t="s">
         <v>50</v>
       </c>
@@ -2691,7 +2703,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="42">
-      <c r="A41" s="86"/>
+      <c r="A41" s="59"/>
       <c r="B41" s="4" t="s">
         <v>51</v>
       </c>
@@ -2723,7 +2735,27 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="36">
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I2:I4"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="G11:J11"/>
@@ -2737,28 +2769,9 @@
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="I2:I4"/>
     <mergeCell ref="B27:B36"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="A11:A25"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[pinghe] #637 add Requested quantity and Authorised quantity to Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/static/requisition/MTB_pt.xlsx
+++ b/src/main/resources/static/requisition/MTB_pt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fubo.ding/projects_siglus_to14/siglus-api/src/main/resources/static/requisition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinghe/Desktop/dev/siglus-api/src/main/resources/static/requisition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53E27E9-4FBE-4E41-A54D-9D2763ECBAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794DCA39-F9F2-6143-8FEE-7E1FCBFE7875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="500" windowWidth="34500" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="1940" windowWidth="34500" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MTB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="137">
   <si>
     <r>
       <rPr>
@@ -442,196 +442,206 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
+    <t>{newSection0new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection0newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection0newColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection0total}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection1new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection1newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection1total}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn2}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn3}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn4}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn5}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection2newColumn6}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn2}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn3}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn4}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection3newColumn6}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4new}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn2}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn3}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn4}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{newSection4newColumn6}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenew}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn0}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn1}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn2}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn3}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypenewColumn4}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{patientTypetotal}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{criança &gt; 25Kgprophylaxis}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{criança &gt; 25Kgtreatment}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{criança &lt; 25Kgprophylaxis}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{criança &lt; 25Kgtreatment}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{adultosprophylaxis}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{adultostreatment}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{createdDate}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> {authorize}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> {approve}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{comment}</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quantidade Autorizada</t>
+  </si>
+  <si>
     <t>{productLineItem.productInventory}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>{productLineItem.requestedQuantity}</t>
+  </si>
+  <si>
+    <t>{productLineItem.authorizedQuantity}</t>
   </si>
   <si>
     <t>{productLineItem.productExpireDate}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection0new}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection0newColumn0}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection0newColumn1}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection0total}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection1new}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection1newColumn0}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection1total}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection2new}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection2newColumn0}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection2newColumn1}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection2newColumn2}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection2newColumn3}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection2newColumn4}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection2newColumn5}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection2newColumn6}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection3new}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection3newColumn0}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection3newColumn1}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection3newColumn2}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection3newColumn3}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection3newColumn4}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection3newColumn6}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection4new}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection4newColumn0}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection4newColumn1}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection4newColumn2}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection4newColumn3}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection4newColumn4}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{newSection4newColumn6}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{patientTypenew}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{patientTypenewColumn0}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{patientTypenewColumn1}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{patientTypenewColumn2}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{patientTypenewColumn3}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{patientTypenewColumn4}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{patientTypetotal}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{criança &gt; 25Kgprophylaxis}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{criança &gt; 25Kgtreatment}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{criança &lt; 25Kgprophylaxis}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{criança &lt; 25Kgtreatment}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{adultosprophylaxis}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{adultostreatment}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{createdDate}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> {authorize}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> {approve}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>{comment}</t>
-    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quantidade Requisitada</t>
   </si>
 </sst>
 </file>
@@ -812,7 +822,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1133,28 +1143,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1263,7 +1251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1297,25 +1285,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1345,37 +1327,37 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1429,13 +1411,13 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1465,13 +1447,13 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1492,7 +1474,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1510,7 +1510,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1519,52 +1519,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1573,15 +1537,33 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1685,9 +1667,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1725,9 +1707,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1760,26 +1742,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1812,26 +1777,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2007,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -2024,714 +1972,727 @@
     <col min="9" max="9" width="12.59765625" customWidth="1"/>
     <col min="10" max="10" width="22.3984375" customWidth="1"/>
     <col min="11" max="11" width="23.59765625" customWidth="1"/>
+    <col min="12" max="12" width="19.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="42" customHeight="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="83" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="50" t="s">
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="49" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.5" customHeight="1">
-      <c r="A2" s="80"/>
+      <c r="A2" s="84"/>
       <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="88" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="85" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.5" customHeight="1">
-      <c r="A3" s="80"/>
+      <c r="A3" s="84"/>
       <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
     </row>
     <row r="4" spans="1:11" ht="14" customHeight="1">
-      <c r="A4" s="80"/>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="84"/>
+      <c r="B4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A5" s="76"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="78"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="82"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" customHeight="1">
-      <c r="B6" s="12"/>
-      <c r="C6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="57"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="55"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" customHeight="1">
-      <c r="B7" s="11"/>
-      <c r="C7" s="7" t="s">
+      <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>34</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="19.5" customHeight="1">
-      <c r="C8" s="49" t="s">
+      <c r="A8" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="B8" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="C8" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="D8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="49" t="s">
+      <c r="E8" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="49" t="s">
+      <c r="F8" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="I8" s="49" t="s">
+      <c r="G8" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="J8" s="53" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28" customHeight="1">
+      <c r="A11" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="93" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="93"/>
+      <c r="D11" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="G11" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="22"/>
+    </row>
+    <row r="12" spans="1:11" ht="14" customHeight="1">
+      <c r="A12" s="79"/>
+      <c r="B12" s="97" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="G12" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="69"/>
+      <c r="J12" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="1:11" ht="13" customHeight="1">
+      <c r="A13" s="79"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="31"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="71"/>
+      <c r="J13" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:11" ht="13" customHeight="1">
+      <c r="A14" s="79"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="71"/>
+      <c r="J14" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:11" ht="13" customHeight="1">
+      <c r="A15" s="79"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="31"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="71"/>
+      <c r="J15" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="1:11" ht="13" customHeight="1">
+      <c r="A16" s="79"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="31"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="71"/>
+      <c r="J16" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:11" ht="13" customHeight="1">
+      <c r="A17" s="79"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="31"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="71"/>
+      <c r="J17" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="1:11" ht="13" customHeight="1">
+      <c r="A18" s="79"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="31"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="77" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="78"/>
+      <c r="J18" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="1:11" ht="13" customHeight="1">
+      <c r="A19" s="79"/>
+      <c r="B19" s="100" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="31"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" ht="13" customHeight="1">
+      <c r="A20" s="79"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="31"/>
+      <c r="G20" s="26"/>
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="1:11" ht="13" customHeight="1">
+      <c r="A21" s="79"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="31"/>
+      <c r="G21" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="69"/>
+      <c r="J21" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="1:11" ht="13" customHeight="1">
+      <c r="A22" s="79"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="31"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="71"/>
+      <c r="J22" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" ht="13" customHeight="1">
+      <c r="A23" s="79"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="31"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="71"/>
+      <c r="J23" s="28" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="28" customHeight="1">
-      <c r="A11" s="94" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="101" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="101"/>
-      <c r="D11" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="G11" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="24"/>
-    </row>
-    <row r="12" spans="1:11" ht="14" customHeight="1">
-      <c r="A12" s="94"/>
-      <c r="B12" s="95" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="E12" s="33"/>
-      <c r="G12" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="48" t="s">
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" ht="13" customHeight="1">
+      <c r="A24" s="79"/>
+      <c r="B24" s="101"/>
+      <c r="C24" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="31"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="71"/>
+      <c r="J24" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" ht="13" customHeight="1">
+      <c r="A25" s="79"/>
+      <c r="B25" s="102"/>
+      <c r="C25" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" s="23"/>
+    </row>
+    <row r="26" spans="1:11" ht="13" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="32"/>
+      <c r="G26" s="26"/>
+      <c r="K26" s="24"/>
+    </row>
+    <row r="27" spans="1:11" ht="13" customHeight="1">
+      <c r="A27" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="33"/>
+      <c r="G27" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27" s="69"/>
+      <c r="J27" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="25"/>
-    </row>
-    <row r="13" spans="1:11" ht="13" customHeight="1">
-      <c r="A13" s="94"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="33"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="75" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="73"/>
-      <c r="J13" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="K13" s="26"/>
-    </row>
-    <row r="14" spans="1:11" ht="13" customHeight="1">
-      <c r="A14" s="94"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="33"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="75" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="73"/>
-      <c r="J14" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="K14" s="26"/>
-    </row>
-    <row r="15" spans="1:11" ht="13" customHeight="1">
-      <c r="A15" s="94"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" s="33"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="73"/>
-      <c r="J15" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="K15" s="26"/>
-    </row>
-    <row r="16" spans="1:11" ht="13" customHeight="1">
-      <c r="A16" s="94"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="I16" s="73"/>
-      <c r="J16" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="K16" s="26"/>
-    </row>
-    <row r="17" spans="1:11" ht="13" customHeight="1">
-      <c r="A17" s="94"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="33"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="75" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="73"/>
-      <c r="J17" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="K17" s="26"/>
-    </row>
-    <row r="18" spans="1:11" ht="13" customHeight="1">
-      <c r="A18" s="94"/>
-      <c r="B18" s="97"/>
-      <c r="C18" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="33"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" s="93"/>
-      <c r="J18" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="K18" s="26"/>
-    </row>
-    <row r="19" spans="1:11" ht="13" customHeight="1">
-      <c r="A19" s="94"/>
-      <c r="B19" s="98" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="K19" s="26"/>
-    </row>
-    <row r="20" spans="1:11" ht="13" customHeight="1">
-      <c r="A20" s="94"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" s="33"/>
-      <c r="G20" s="28"/>
-      <c r="K20" s="25"/>
-    </row>
-    <row r="21" spans="1:11" ht="13" customHeight="1">
-      <c r="A21" s="94"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="33"/>
-      <c r="G21" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="I21" s="71"/>
-      <c r="J21" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="26"/>
-    </row>
-    <row r="22" spans="1:11" ht="13" customHeight="1">
-      <c r="A22" s="94"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="33"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="75" t="s">
-        <v>64</v>
-      </c>
-      <c r="I22" s="73"/>
-      <c r="J22" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="K22" s="26"/>
-    </row>
-    <row r="23" spans="1:11" ht="13" customHeight="1">
-      <c r="A23" s="94"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="33"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23" s="73"/>
-      <c r="J23" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="K23" s="26"/>
-    </row>
-    <row r="24" spans="1:11" ht="13" customHeight="1">
-      <c r="A24" s="94"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="E24" s="33"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="75" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="73"/>
-      <c r="J24" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="K24" s="26"/>
-    </row>
-    <row r="25" spans="1:11" ht="13" customHeight="1">
-      <c r="A25" s="94"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="33"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J25" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="K25" s="25"/>
-    </row>
-    <row r="26" spans="1:11" ht="13" customHeight="1">
-      <c r="A26" s="46"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="34"/>
-      <c r="G26" s="28"/>
-      <c r="K26" s="26"/>
-    </row>
-    <row r="27" spans="1:11" ht="13" customHeight="1">
-      <c r="A27" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="89" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="35"/>
-      <c r="G27" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="H27" s="70" t="s">
-        <v>67</v>
-      </c>
-      <c r="I27" s="71"/>
-      <c r="J27" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27" s="26"/>
+      <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:11" ht="13" customHeight="1">
-      <c r="A28" s="59"/>
-      <c r="B28" s="90"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="75"/>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="33"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="31"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="73"/>
-      <c r="J28" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="K28" s="26"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:11" ht="13" customHeight="1">
-      <c r="A29" s="59"/>
-      <c r="B29" s="90"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="75"/>
       <c r="C29" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="33"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="31"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="73"/>
-      <c r="J29" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="K29" s="25"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="K29" s="23"/>
     </row>
     <row r="30" spans="1:11" ht="13" customHeight="1">
-      <c r="A30" s="59"/>
-      <c r="B30" s="90"/>
-      <c r="C30" s="21" t="s">
+      <c r="A30" s="57"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="18"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="34"/>
+      <c r="F30" s="16"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="31" t="s">
-        <v>93</v>
+      <c r="J30" s="29" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="13" customHeight="1">
-      <c r="A31" s="59"/>
-      <c r="B31" s="90"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="75"/>
       <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" s="33"/>
-      <c r="F31" s="18"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="E31" s="31"/>
+      <c r="F31" s="16"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="1:11" ht="13" customHeight="1">
-      <c r="A32" s="59"/>
-      <c r="B32" s="90"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="31"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="69"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="67"/>
     </row>
     <row r="33" spans="1:10" ht="13" customHeight="1">
-      <c r="A33" s="59"/>
-      <c r="B33" s="90"/>
+      <c r="A33" s="57"/>
+      <c r="B33" s="75"/>
       <c r="C33" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" s="33"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="104" t="s">
-        <v>132</v>
-      </c>
-      <c r="H33" s="103"/>
-      <c r="I33" s="103"/>
-      <c r="J33" s="103"/>
+        <v>97</v>
+      </c>
+      <c r="E33" s="31"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="95" t="s">
+        <v>130</v>
+      </c>
+      <c r="H33" s="96"/>
+      <c r="I33" s="96"/>
+      <c r="J33" s="96"/>
     </row>
     <row r="34" spans="1:10" ht="13" customHeight="1">
-      <c r="A34" s="59"/>
-      <c r="B34" s="90"/>
+      <c r="A34" s="57"/>
+      <c r="B34" s="75"/>
       <c r="C34" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
+        <v>98</v>
+      </c>
+      <c r="E34" s="31"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
     </row>
     <row r="35" spans="1:10" ht="13" customHeight="1">
-      <c r="A35" s="59"/>
-      <c r="B35" s="90"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="75"/>
       <c r="C35" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E35" s="33"/>
-      <c r="F35" s="18"/>
+        <v>99</v>
+      </c>
+      <c r="E35" s="31"/>
+      <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:10" ht="13" customHeight="1">
-      <c r="A36" s="102"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="20"/>
+      <c r="A36" s="94"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="18"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="16"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="19"/>
-      <c r="F37" s="18"/>
+      <c r="A37" s="17"/>
+      <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:10" ht="29" customHeight="1">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="42" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="14" customHeight="1">
-      <c r="A39" s="59"/>
+      <c r="A39" s="57"/>
       <c r="B39" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="45" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="14" customHeight="1">
-      <c r="A40" s="59"/>
+      <c r="A40" s="57"/>
       <c r="B40" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D40" s="45" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+      <c r="D40" s="43" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="42">
-      <c r="A41" s="59"/>
+      <c r="A41" s="57"/>
       <c r="B41" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" s="45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="47" customFormat="1" ht="28">
-      <c r="A43" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" s="43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="45" customFormat="1" ht="28">
+      <c r="A43" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="52" t="s">
-        <v>130</v>
-      </c>
-      <c r="D43" s="52" t="s">
+      <c r="B43" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="E43" s="52" t="s">
-        <v>131</v>
-      </c>
-      <c r="G43" s="53" t="s">
+      <c r="E43" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="G43" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="H43" s="54" t="s">
-        <v>129</v>
+      <c r="H43" s="52" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2756,7 +2717,7 @@
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I2:I4"/>
-    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="A6:J6"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:G18"/>

</xml_diff>

<commit_message>
[pinghe] #637 update excel
</commit_message>
<xml_diff>
--- a/src/main/resources/static/requisition/MTB_pt.xlsx
+++ b/src/main/resources/static/requisition/MTB_pt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinghe/Desktop/dev/siglus-api/src/main/resources/static/requisition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794DCA39-F9F2-6143-8FEE-7E1FCBFE7875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF421A1D-98B6-CC42-A9A9-1ECA5168357E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="1940" windowWidth="34500" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="139">
   <si>
     <r>
       <rPr>
@@ -642,6 +642,12 @@
   </si>
   <si>
     <t>Quantidade Requisitada</t>
+  </si>
+  <si>
+    <t>Quantidade Aprovada</t>
+  </si>
+  <si>
+    <t>{productLineItem.approvedQuantity}</t>
   </si>
 </sst>
 </file>
@@ -1133,17 +1139,6 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -1242,6 +1237,21 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1291,13 +1301,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1327,7 +1337,7 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1342,22 +1352,22 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1414,18 +1424,93 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1447,33 +1532,21 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1492,73 +1565,10 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1955,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -1976,20 +1986,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="42" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="73" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="88"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="48" t="s">
         <v>26</v>
       </c>
@@ -1998,82 +2008,83 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.5" customHeight="1">
-      <c r="A2" s="84"/>
+      <c r="A2" s="74"/>
       <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="92" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="85" t="s">
+      <c r="J2" s="75" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.5" customHeight="1">
-      <c r="A3" s="84"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
     </row>
     <row r="4" spans="1:11" ht="14" customHeight="1">
-      <c r="A4" s="84"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="89"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A5" s="80"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="82"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" customHeight="1">
       <c r="A7" s="7" t="s">
@@ -2106,6 +2117,9 @@
       <c r="J7" s="5" t="s">
         <v>131</v>
       </c>
+      <c r="K7" s="102" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="19.5" customHeight="1">
       <c r="A8" s="47" t="s">
@@ -2138,30 +2152,33 @@
       <c r="J8" s="53" t="s">
         <v>134</v>
       </c>
+      <c r="K8" s="53" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="28" customHeight="1">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="93"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="39" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="30"/>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="60"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="85"/>
       <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" ht="14" customHeight="1">
-      <c r="A12" s="79"/>
-      <c r="B12" s="97" t="s">
+      <c r="A12" s="100"/>
+      <c r="B12" s="61" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="38" t="s">
@@ -2171,10 +2188,10 @@
         <v>100</v>
       </c>
       <c r="E12" s="31"/>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="72" t="s">
+      <c r="H12" s="68" t="s">
         <v>56</v>
       </c>
       <c r="I12" s="69"/>
@@ -2184,8 +2201,8 @@
       <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" ht="13" customHeight="1">
-      <c r="A13" s="79"/>
-      <c r="B13" s="98"/>
+      <c r="A13" s="100"/>
+      <c r="B13" s="62"/>
       <c r="C13" s="38" t="s">
         <v>2</v>
       </c>
@@ -2193,19 +2210,19 @@
         <v>106</v>
       </c>
       <c r="E13" s="31"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="73" t="s">
+      <c r="G13" s="87"/>
+      <c r="H13" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="71"/>
+      <c r="I13" s="58"/>
       <c r="J13" s="28" t="s">
         <v>114</v>
       </c>
       <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:11" ht="13" customHeight="1">
-      <c r="A14" s="79"/>
-      <c r="B14" s="98"/>
+      <c r="A14" s="100"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="38" t="s">
         <v>3</v>
       </c>
@@ -2213,19 +2230,19 @@
         <v>101</v>
       </c>
       <c r="E14" s="31"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="73" t="s">
+      <c r="G14" s="87"/>
+      <c r="H14" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="71"/>
+      <c r="I14" s="58"/>
       <c r="J14" s="28" t="s">
         <v>115</v>
       </c>
       <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" ht="13" customHeight="1">
-      <c r="A15" s="79"/>
-      <c r="B15" s="98"/>
+      <c r="A15" s="100"/>
+      <c r="B15" s="62"/>
       <c r="C15" s="38" t="s">
         <v>4</v>
       </c>
@@ -2233,19 +2250,19 @@
         <v>102</v>
       </c>
       <c r="E15" s="31"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="73" t="s">
+      <c r="G15" s="87"/>
+      <c r="H15" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="71"/>
+      <c r="I15" s="58"/>
       <c r="J15" s="28" t="s">
         <v>116</v>
       </c>
       <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1">
-      <c r="A16" s="79"/>
-      <c r="B16" s="98"/>
+      <c r="A16" s="100"/>
+      <c r="B16" s="62"/>
       <c r="C16" s="38" t="s">
         <v>5</v>
       </c>
@@ -2253,19 +2270,19 @@
         <v>103</v>
       </c>
       <c r="E16" s="31"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="73" t="s">
+      <c r="G16" s="87"/>
+      <c r="H16" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="71"/>
+      <c r="I16" s="58"/>
       <c r="J16" s="28" t="s">
         <v>117</v>
       </c>
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11" ht="13" customHeight="1">
-      <c r="A17" s="79"/>
-      <c r="B17" s="98"/>
+      <c r="A17" s="100"/>
+      <c r="B17" s="62"/>
       <c r="C17" s="38" t="s">
         <v>6</v>
       </c>
@@ -2273,19 +2290,19 @@
         <v>104</v>
       </c>
       <c r="E17" s="31"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="73" t="s">
+      <c r="G17" s="87"/>
+      <c r="H17" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="71"/>
+      <c r="I17" s="58"/>
       <c r="J17" s="28" t="s">
         <v>118</v>
       </c>
       <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:11" ht="13" customHeight="1">
-      <c r="A18" s="79"/>
-      <c r="B18" s="99"/>
+      <c r="A18" s="100"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="38" t="s">
         <v>7</v>
       </c>
@@ -2293,19 +2310,19 @@
         <v>105</v>
       </c>
       <c r="E18" s="31"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="77" t="s">
+      <c r="G18" s="88"/>
+      <c r="H18" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="78"/>
+      <c r="I18" s="99"/>
       <c r="J18" s="28" t="s">
         <v>119</v>
       </c>
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" ht="13" customHeight="1">
-      <c r="A19" s="79"/>
-      <c r="B19" s="100" t="s">
+      <c r="A19" s="100"/>
+      <c r="B19" s="64" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="37" t="s">
@@ -2326,8 +2343,8 @@
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" ht="13" customHeight="1">
-      <c r="A20" s="79"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="100"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="37" t="s">
         <v>2</v>
       </c>
@@ -2339,8 +2356,8 @@
       <c r="K20" s="23"/>
     </row>
     <row r="21" spans="1:11" ht="13" customHeight="1">
-      <c r="A21" s="79"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="100"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="37" t="s">
         <v>3</v>
       </c>
@@ -2348,10 +2365,10 @@
         <v>108</v>
       </c>
       <c r="E21" s="31"/>
-      <c r="G21" s="61" t="s">
+      <c r="G21" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="72" t="s">
+      <c r="H21" s="68" t="s">
         <v>57</v>
       </c>
       <c r="I21" s="69"/>
@@ -2361,8 +2378,8 @@
       <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" ht="13" customHeight="1">
-      <c r="A22" s="79"/>
-      <c r="B22" s="101"/>
+      <c r="A22" s="100"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="37" t="s">
         <v>4</v>
       </c>
@@ -2370,19 +2387,19 @@
         <v>109</v>
       </c>
       <c r="E22" s="31"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="73" t="s">
+      <c r="G22" s="87"/>
+      <c r="H22" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="I22" s="71"/>
+      <c r="I22" s="58"/>
       <c r="J22" s="28" t="s">
         <v>85</v>
       </c>
       <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" ht="13" customHeight="1">
-      <c r="A23" s="79"/>
-      <c r="B23" s="101"/>
+      <c r="A23" s="100"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="37" t="s">
         <v>5</v>
       </c>
@@ -2390,19 +2407,19 @@
         <v>110</v>
       </c>
       <c r="E23" s="31"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="73" t="s">
+      <c r="G23" s="87"/>
+      <c r="H23" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="I23" s="71"/>
+      <c r="I23" s="58"/>
       <c r="J23" s="28" t="s">
         <v>86</v>
       </c>
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" ht="13" customHeight="1">
-      <c r="A24" s="79"/>
-      <c r="B24" s="101"/>
+      <c r="A24" s="100"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="37" t="s">
         <v>7</v>
       </c>
@@ -2410,19 +2427,19 @@
         <v>111</v>
       </c>
       <c r="E24" s="31"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="73" t="s">
+      <c r="G24" s="87"/>
+      <c r="H24" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="I24" s="71"/>
+      <c r="I24" s="58"/>
       <c r="J24" s="28" t="s">
         <v>87</v>
       </c>
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" ht="13" customHeight="1">
-      <c r="A25" s="79"/>
-      <c r="B25" s="102"/>
+      <c r="A25" s="100"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="37" t="s">
         <v>8</v>
       </c>
@@ -2450,10 +2467,10 @@
       <c r="K26" s="24"/>
     </row>
     <row r="27" spans="1:11" ht="13" customHeight="1">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="95" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="40" t="s">
@@ -2463,10 +2480,10 @@
         <v>44</v>
       </c>
       <c r="E27" s="33"/>
-      <c r="G27" s="64" t="s">
+      <c r="G27" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="68" t="s">
+      <c r="H27" s="93" t="s">
         <v>67</v>
       </c>
       <c r="I27" s="69"/>
@@ -2476,8 +2493,8 @@
       <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:11" ht="13" customHeight="1">
-      <c r="A28" s="57"/>
-      <c r="B28" s="75"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="96"/>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
@@ -2485,19 +2502,19 @@
         <v>92</v>
       </c>
       <c r="E28" s="31"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="70" t="s">
+      <c r="G28" s="89"/>
+      <c r="H28" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="71"/>
+      <c r="I28" s="58"/>
       <c r="J28" s="28" t="s">
         <v>89</v>
       </c>
       <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:11" ht="13" customHeight="1">
-      <c r="A29" s="57"/>
-      <c r="B29" s="75"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="96"/>
       <c r="C29" s="4" t="s">
         <v>10</v>
       </c>
@@ -2505,19 +2522,19 @@
         <v>93</v>
       </c>
       <c r="E29" s="31"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="70" t="s">
+      <c r="G29" s="89"/>
+      <c r="H29" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="71"/>
+      <c r="I29" s="58"/>
       <c r="J29" s="28" t="s">
         <v>90</v>
       </c>
       <c r="K29" s="23"/>
     </row>
     <row r="30" spans="1:11" ht="13" customHeight="1">
-      <c r="A30" s="57"/>
-      <c r="B30" s="75"/>
+      <c r="A30" s="55"/>
+      <c r="B30" s="96"/>
       <c r="C30" s="19" t="s">
         <v>11</v>
       </c>
@@ -2535,8 +2552,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="13" customHeight="1">
-      <c r="A31" s="57"/>
-      <c r="B31" s="75"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="96"/>
       <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
@@ -2550,8 +2567,8 @@
       <c r="J31" s="21"/>
     </row>
     <row r="32" spans="1:11" ht="13" customHeight="1">
-      <c r="A32" s="57"/>
-      <c r="B32" s="75"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="96"/>
       <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
@@ -2560,16 +2577,16 @@
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="16"/>
-      <c r="G32" s="65" t="s">
+      <c r="G32" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="67"/>
+      <c r="H32" s="91"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="92"/>
     </row>
     <row r="33" spans="1:10" ht="13" customHeight="1">
-      <c r="A33" s="57"/>
-      <c r="B33" s="75"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="96"/>
       <c r="C33" s="4" t="s">
         <v>14</v>
       </c>
@@ -2578,16 +2595,16 @@
       </c>
       <c r="E33" s="31"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="95" t="s">
+      <c r="G33" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="H33" s="96"/>
-      <c r="I33" s="96"/>
-      <c r="J33" s="96"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
     </row>
     <row r="34" spans="1:10" ht="13" customHeight="1">
-      <c r="A34" s="57"/>
-      <c r="B34" s="75"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="96"/>
       <c r="C34" s="4" t="s">
         <v>15</v>
       </c>
@@ -2602,8 +2619,8 @@
       <c r="J34" s="16"/>
     </row>
     <row r="35" spans="1:10" ht="13" customHeight="1">
-      <c r="A35" s="57"/>
-      <c r="B35" s="75"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="96"/>
       <c r="C35" s="4" t="s">
         <v>16</v>
       </c>
@@ -2614,8 +2631,8 @@
       <c r="F35" s="16"/>
     </row>
     <row r="36" spans="1:10" ht="13" customHeight="1">
-      <c r="A36" s="94"/>
-      <c r="B36" s="76"/>
+      <c r="A36" s="56"/>
+      <c r="B36" s="97"/>
       <c r="C36" s="18"/>
       <c r="D36" s="3"/>
       <c r="E36" s="35"/>
@@ -2626,7 +2643,7 @@
       <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:10" ht="29" customHeight="1">
-      <c r="A38" s="56" t="s">
+      <c r="A38" s="54" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="40" t="s">
@@ -2640,7 +2657,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="14" customHeight="1">
-      <c r="A39" s="57"/>
+      <c r="A39" s="55"/>
       <c r="B39" s="4" t="s">
         <v>49</v>
       </c>
@@ -2652,7 +2669,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="14" customHeight="1">
-      <c r="A40" s="57"/>
+      <c r="A40" s="55"/>
       <c r="B40" s="4" t="s">
         <v>50</v>
       </c>
@@ -2664,7 +2681,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="42">
-      <c r="A41" s="57"/>
+      <c r="A41" s="55"/>
       <c r="B41" s="4" t="s">
         <v>51</v>
       </c>
@@ -2697,27 +2714,7 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:G18"/>
@@ -2733,6 +2730,26 @@
     <mergeCell ref="B27:B36"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="A11:A25"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B19:B25"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>